<commit_message>
One sheet per student
</commit_message>
<xml_diff>
--- a/gabarits_grilles/grille_5_niveaux.xlsx
+++ b/gabarits_grilles/grille_5_niveaux.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varchambaultbouffard\Git_archambaultv-prof\c3hm\gabarits_grilles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8067BF21-A8CD-4DE0-819F-C004D7BE989C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A012A884-C738-4210-9300-41B54571752C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="3705" windowWidth="33975" windowHeight="16425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7905" yWindow="5730" windowWidth="25530" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="c3hm" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="cthm_code_omnivox">'c3hm'!$A$1</definedName>
-    <definedName name="cthm_config_key">'c3hm'!$E$1</definedName>
+    <definedName name="cthm_config_key">'c3hm'!$F$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="104">
   <si>
     <t>Excellent</t>
   </si>
@@ -337,6 +337,18 @@
   </si>
   <si>
     <t>Nombre de décimales pour le total et les poids des critères ou les seuils.</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Vin</t>
+  </si>
+  <si>
+    <t>Mig</t>
+  </si>
+  <si>
+    <t>Car</t>
   </si>
 </sst>
 </file>
@@ -494,10 +506,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6DAE6ADB-19E4-4BDA-A984-C82CBEC06937}" name="cthm_tableau_desc_cle3" displayName="cthm_tableau_desc_cle3" ref="I2:J12" totalsRowShown="0" dataDxfId="2">
-  <autoFilter ref="I2:J12" xr:uid="{6DAE6ADB-19E4-4BDA-A984-C82CBEC06937}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I3:J11">
-    <sortCondition ref="I2:I11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6DAE6ADB-19E4-4BDA-A984-C82CBEC06937}" name="cthm_tableau_desc_cle3" displayName="cthm_tableau_desc_cle3" ref="J2:K12" totalsRowShown="0" dataDxfId="2">
+  <autoFilter ref="J2:K12" xr:uid="{6DAE6ADB-19E4-4BDA-A984-C82CBEC06937}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="J3:K11">
+    <sortCondition ref="J2:J11"/>
   </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{E0C7F19B-0EC8-4B89-81EA-3CCBB78F2E23}" name="Clé" dataDxfId="1"/>
@@ -792,10 +804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D1A45DF-FA3D-48B6-99B6-DCC84A221081}">
-  <dimension ref="A1:L56"/>
+  <dimension ref="A1:M56"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -803,17 +815,18 @@
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.5703125" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="42.85546875" customWidth="1"/>
-    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.85546875" customWidth="1"/>
-    <col min="10" max="10" width="114.28515625" customWidth="1"/>
-    <col min="12" max="12" width="18.28515625" customWidth="1"/>
-    <col min="13" max="13" width="114.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="3.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42.85546875" customWidth="1"/>
+    <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.85546875" customWidth="1"/>
+    <col min="11" max="11" width="114.28515625" customWidth="1"/>
+    <col min="13" max="13" width="18.28515625" customWidth="1"/>
+    <col min="14" max="14" width="114.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -823,17 +836,20 @@
       <c r="C1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="D1" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>314159</v>
       </c>
@@ -843,20 +859,23 @@
       <c r="C2" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="D2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>14</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>271858</v>
       </c>
@@ -866,20 +885,23 @@
       <c r="C3" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="D3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="G3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="J3" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="K3" s="6" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>141421</v>
       </c>
@@ -889,20 +911,23 @@
       <c r="C4" t="s">
         <v>25</v>
       </c>
-      <c r="E4" t="s">
+      <c r="D4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F4" t="s">
         <v>66</v>
       </c>
-      <c r="F4" s="7">
+      <c r="G4" s="7">
         <v>100</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="J4" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="K4" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>161803</v>
       </c>
@@ -912,485 +937,488 @@
       <c r="C5" t="s">
         <v>28</v>
       </c>
-      <c r="E5" t="s">
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
         <v>97</v>
       </c>
-      <c r="F5" s="7">
+      <c r="G5" s="7">
         <v>0</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="J5" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="K5" s="6" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="E6" s="7" t="s">
+    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="F6" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="G6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="J6" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="K6" s="6" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E7" s="7" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F7" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="G7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="J7" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="K7" s="6" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E8" s="7" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F8" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="G8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="J8" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="J8" s="8" t="s">
+      <c r="K8" s="8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E9" s="7" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F9" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="G9" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="J9" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="K9" s="6" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="E10" s="7" t="s">
+    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="F10" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="G10" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="J10" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="J10" s="6" t="s">
+      <c r="K10" s="6" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="E11" s="7" t="s">
+    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="F11" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="F11" s="7">
+      <c r="G11" s="7">
         <v>100</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="J11" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="J11" s="6" t="s">
+      <c r="K11" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E12" s="7" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F12" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="F12" s="7">
+      <c r="G12" s="7">
         <v>85</v>
       </c>
-      <c r="I12" s="7" t="s">
+      <c r="J12" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="J12" s="6" t="s">
+      <c r="K12" s="6" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E13" s="7" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F13" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="F13" s="7">
+      <c r="G13" s="7">
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E14" s="7" t="s">
+    <row r="14" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F14" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="F14" s="7">
+      <c r="G14" s="7">
         <v>60</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E15" s="7" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F15" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="F15" s="7">
+      <c r="G15" s="7">
         <v>0</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E16" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
         <v>96</v>
       </c>
-      <c r="F16" s="7">
+      <c r="G16" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="5:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E17" s="3" t="s">
+    <row r="17" spans="6:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F17" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="G17" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E18" s="7" t="s">
+    <row r="18" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F18" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>30</v>
       </c>
-      <c r="I18" s="9" t="s">
+      <c r="J18" s="9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="5:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E19" s="2" t="s">
+    <row r="19" spans="6:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F19" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="G19" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="L19" s="1"/>
-    </row>
-    <row r="20" spans="5:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E20" s="1" t="s">
+      <c r="M19" s="1"/>
+    </row>
+    <row r="20" spans="6:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F20" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="G20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="L20" s="9"/>
-    </row>
-    <row r="21" spans="5:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E21" s="1" t="s">
+      <c r="M20" s="9"/>
+    </row>
+    <row r="21" spans="6:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F21" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="5:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E22" s="1" t="s">
+    <row r="22" spans="6:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F22" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="5:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E23" s="1" t="s">
+    <row r="23" spans="6:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F23" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="5:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E24" s="1" t="s">
+    <row r="24" spans="6:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F24" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E25" s="2" t="s">
+    <row r="25" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F25" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="G25" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="5:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E26" s="1" t="s">
+    <row r="26" spans="6:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F26" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="G26" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="5:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E27" s="1" t="s">
+    <row r="27" spans="6:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F27" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="G27" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="5:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E28" s="1" t="s">
+    <row r="28" spans="6:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F28" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="5:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E29" s="1" t="s">
+    <row r="29" spans="6:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F29" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="G29" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="5:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E30" s="1" t="s">
+    <row r="30" spans="6:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F30" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="G30" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E31" s="2" t="s">
+    <row r="31" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F31" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="G31" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="5:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E32" s="1" t="s">
+    <row r="32" spans="6:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F32" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="G32" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="5:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E33" s="1" t="s">
+    <row r="33" spans="6:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F33" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="G33" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="5:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E34" s="1" t="s">
+    <row r="34" spans="6:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F34" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="G34" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="5:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E35" s="1" t="s">
+    <row r="35" spans="6:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F35" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="G35" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="5:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E36" s="1" t="s">
+    <row r="36" spans="6:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F36" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="G36" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="5:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E37" s="3" t="s">
+    <row r="37" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F37" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="G37" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E38" s="7" t="s">
+    <row r="38" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F38" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="F38" s="10"/>
-    </row>
-    <row r="39" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E39" s="2" t="s">
+      <c r="G38" s="10"/>
+    </row>
+    <row r="39" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F39" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="G39" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="5:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E40" s="1" t="s">
+    <row r="40" spans="6:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F40" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="G40" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="41" spans="5:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E41" s="1" t="s">
+    <row r="41" spans="6:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F41" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="G41" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="5:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E42" s="1" t="s">
+    <row r="42" spans="6:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F42" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="G42" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="43" spans="5:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E43" s="1" t="s">
+    <row r="43" spans="6:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F43" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="G43" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="44" spans="5:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E44" s="1" t="s">
+    <row r="44" spans="6:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F44" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="G44" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E45" s="2" t="s">
+    <row r="45" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F45" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F45" s="2" t="s">
+      <c r="G45" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="5:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E46" s="1" t="s">
+    <row r="46" spans="6:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F46" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F46" s="1" t="s">
+      <c r="G46" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="47" spans="5:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E47" s="1" t="s">
+    <row r="47" spans="6:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F47" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="G47" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="48" spans="5:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E48" s="1" t="s">
+    <row r="48" spans="6:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F48" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F48" s="1" t="s">
+      <c r="G48" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="49" spans="5:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E49" s="1" t="s">
+    <row r="49" spans="6:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F49" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F49" s="1" t="s">
+      <c r="G49" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="50" spans="5:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E50" s="1" t="s">
+    <row r="50" spans="6:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F50" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F50" s="1" t="s">
+      <c r="G50" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="51" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E51" s="2" t="s">
+    <row r="51" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F51" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F51" s="2" t="s">
+      <c r="G51" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="5:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E52" s="1" t="s">
+    <row r="52" spans="6:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F52" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F52" s="1" t="s">
+      <c r="G52" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="53" spans="5:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E53" s="1" t="s">
+    <row r="53" spans="6:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F53" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F53" s="1" t="s">
+      <c r="G53" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="54" spans="5:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E54" s="1" t="s">
+    <row r="54" spans="6:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F54" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F54" s="1" t="s">
+      <c r="G54" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="55" spans="5:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E55" s="1" t="s">
+    <row r="55" spans="6:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F55" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F55" s="1" t="s">
+      <c r="G55" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="56" spans="5:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E56" s="1" t="s">
+    <row r="56" spans="6:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F56" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F56" s="1" t="s">
+      <c r="G56" s="1" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="I18" r:id="rId1" xr:uid="{B5A7BA30-B542-4287-8813-496D32A71405}"/>
+    <hyperlink ref="J18" r:id="rId1" xr:uid="{B5A7BA30-B542-4287-8813-496D32A71405}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>